<commit_message>
organizei os dados de leitura
</commit_message>
<xml_diff>
--- a/Dados 2018/dataset_export/prograd_to_merge.xlsx
+++ b/Dados 2018/dataset_export/prograd_to_merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="301">
   <si>
     <t>Estudante</t>
   </si>
@@ -412,28 +412,28 @@
     <t>CPTL</t>
   </si>
   <si>
-    <t>Faed</t>
-  </si>
-  <si>
-    <t>Facfan</t>
-  </si>
-  <si>
-    <t>Faodo</t>
+    <t>FAED</t>
+  </si>
+  <si>
+    <t>FACFAN</t>
+  </si>
+  <si>
+    <t>FAODO</t>
   </si>
   <si>
     <t>CPPP</t>
   </si>
   <si>
-    <t>Inqui</t>
-  </si>
-  <si>
-    <t>Faeng</t>
-  </si>
-  <si>
-    <t>Infi</t>
-  </si>
-  <si>
-    <t>Facom</t>
+    <t>INQUI</t>
+  </si>
+  <si>
+    <t>FAENG</t>
+  </si>
+  <si>
+    <t>INFI</t>
+  </si>
+  <si>
+    <t>FACOM</t>
   </si>
   <si>
     <t>CPAQ</t>
@@ -448,25 +448,19 @@
     <t>FAMED</t>
   </si>
   <si>
-    <t>FAMED/ INISA</t>
+    <t>FAMED/INISA</t>
   </si>
   <si>
     <t>INISA</t>
   </si>
   <si>
-    <t>FACFAN</t>
-  </si>
-  <si>
     <t>CPCS</t>
   </si>
   <si>
-    <t>Famez</t>
+    <t>FAMEZ</t>
   </si>
   <si>
     <t>CPNV</t>
-  </si>
-  <si>
-    <t>FAED</t>
   </si>
   <si>
     <t>FAALC</t>
@@ -1308,10 +1302,10 @@
         <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1322,10 +1316,10 @@
         <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1336,10 +1330,10 @@
         <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1350,10 +1344,10 @@
         <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1364,10 +1358,10 @@
         <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1378,10 +1372,10 @@
         <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1392,10 +1386,10 @@
         <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1406,10 +1400,10 @@
         <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1420,10 +1414,10 @@
         <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1434,10 +1428,10 @@
         <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1448,10 +1442,10 @@
         <v>133</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1462,10 +1456,10 @@
         <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1476,10 +1470,10 @@
         <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1490,10 +1484,10 @@
         <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1504,10 +1498,10 @@
         <v>133</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1518,10 +1512,10 @@
         <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1532,10 +1526,10 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1546,10 +1540,10 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1560,10 +1554,10 @@
         <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1574,10 +1568,10 @@
         <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1588,10 +1582,10 @@
         <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1602,10 +1596,10 @@
         <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1616,10 +1610,10 @@
         <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1630,10 +1624,10 @@
         <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1644,10 +1638,10 @@
         <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1658,10 +1652,10 @@
         <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1672,10 +1666,10 @@
         <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1686,10 +1680,10 @@
         <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1700,10 +1694,10 @@
         <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1714,10 +1708,10 @@
         <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D31" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1728,10 +1722,10 @@
         <v>135</v>
       </c>
       <c r="C32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1742,10 +1736,10 @@
         <v>137</v>
       </c>
       <c r="C33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1756,10 +1750,10 @@
         <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D34" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1770,10 +1764,10 @@
         <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D35" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1784,10 +1778,10 @@
         <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D36" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1798,10 +1792,10 @@
         <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1812,10 +1806,10 @@
         <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1826,10 +1820,10 @@
         <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D39" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1840,10 +1834,10 @@
         <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D40" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1854,10 +1848,10 @@
         <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D41" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1868,10 +1862,10 @@
         <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1882,10 +1876,10 @@
         <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D43" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1896,10 +1890,10 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D44" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1910,10 +1904,10 @@
         <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D45" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1924,10 +1918,10 @@
         <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1938,10 +1932,10 @@
         <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D47" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1952,10 +1946,10 @@
         <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1966,10 +1960,10 @@
         <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D49" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1980,10 +1974,10 @@
         <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D50" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1994,10 +1988,10 @@
         <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D51" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2008,10 +2002,10 @@
         <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2022,10 +2016,10 @@
         <v>139</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2036,10 +2030,10 @@
         <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D54" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2050,10 +2044,10 @@
         <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D55" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2064,10 +2058,10 @@
         <v>140</v>
       </c>
       <c r="C56" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2078,10 +2072,10 @@
         <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D57" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2092,10 +2086,10 @@
         <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D58" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2106,10 +2100,10 @@
         <v>141</v>
       </c>
       <c r="C59" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2120,10 +2114,10 @@
         <v>135</v>
       </c>
       <c r="C60" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D60" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2134,10 +2128,10 @@
         <v>137</v>
       </c>
       <c r="C61" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D61" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2148,10 +2142,10 @@
         <v>135</v>
       </c>
       <c r="C62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D62" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2162,10 +2156,10 @@
         <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D63" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2176,10 +2170,10 @@
         <v>135</v>
       </c>
       <c r="C64" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D64" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2190,10 +2184,10 @@
         <v>135</v>
       </c>
       <c r="C65" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D65" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2204,10 +2198,10 @@
         <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D66" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2218,10 +2212,10 @@
         <v>135</v>
       </c>
       <c r="C67" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D67" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2232,10 +2226,10 @@
         <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D68" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2246,10 +2240,10 @@
         <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D69" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2260,10 +2254,10 @@
         <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D70" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2274,10 +2268,10 @@
         <v>143</v>
       </c>
       <c r="C71" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2288,10 +2282,10 @@
         <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D72" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2302,10 +2296,10 @@
         <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D73" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2316,10 +2310,10 @@
         <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D74" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2327,13 +2321,13 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D75" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2344,10 +2338,10 @@
         <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D76" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2358,10 +2352,10 @@
         <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2372,10 +2366,10 @@
         <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D78" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2383,13 +2377,13 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C79" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D79" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2397,13 +2391,13 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C80" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D80" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2411,13 +2405,13 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D81" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2425,13 +2419,13 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C82" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D82" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2439,13 +2433,13 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D83" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2453,13 +2447,13 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C84" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D84" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2467,13 +2461,13 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D85" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2481,13 +2475,13 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D86" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2495,13 +2489,13 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C87" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D87" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2509,13 +2503,13 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C88" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D88" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2523,13 +2517,13 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C89" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D89" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2540,10 +2534,10 @@
         <v>131</v>
       </c>
       <c r="C90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D90" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2554,10 +2548,10 @@
         <v>131</v>
       </c>
       <c r="C91" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D91" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2568,10 +2562,10 @@
         <v>131</v>
       </c>
       <c r="C92" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D92" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2582,10 +2576,10 @@
         <v>131</v>
       </c>
       <c r="C93" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D93" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2596,10 +2590,10 @@
         <v>131</v>
       </c>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D94" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2610,10 +2604,10 @@
         <v>131</v>
       </c>
       <c r="C95" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D95" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2624,10 +2618,10 @@
         <v>131</v>
       </c>
       <c r="C96" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D96" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2638,10 +2632,10 @@
         <v>131</v>
       </c>
       <c r="C97" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D97" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2649,13 +2643,13 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D98" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2663,13 +2657,13 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D99" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2677,13 +2671,13 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C100" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D100" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2691,13 +2685,13 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C101" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D101" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2705,13 +2699,13 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C102" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D102" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2722,10 +2716,10 @@
         <v>142</v>
       </c>
       <c r="C103" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D103" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2736,10 +2730,10 @@
         <v>142</v>
       </c>
       <c r="C104" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D104" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2750,10 +2744,10 @@
         <v>142</v>
       </c>
       <c r="C105" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D105" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2764,10 +2758,10 @@
         <v>142</v>
       </c>
       <c r="C106" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D106" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2778,10 +2772,10 @@
         <v>141</v>
       </c>
       <c r="C107" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D107" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2792,10 +2786,10 @@
         <v>142</v>
       </c>
       <c r="C108" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D108" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2806,10 +2800,10 @@
         <v>142</v>
       </c>
       <c r="C109" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D109" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2820,10 +2814,10 @@
         <v>142</v>
       </c>
       <c r="C110" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D110" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2831,13 +2825,13 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D111" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2845,13 +2839,13 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D112" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2862,10 +2856,10 @@
         <v>131</v>
       </c>
       <c r="C113" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D113" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2873,13 +2867,13 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C114" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D114" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2887,13 +2881,13 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C115" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D115" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2901,13 +2895,13 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C116" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D116" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2918,10 +2912,10 @@
         <v>142</v>
       </c>
       <c r="C117" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D117" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2932,10 +2926,10 @@
         <v>142</v>
       </c>
       <c r="C118" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D118" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2946,10 +2940,10 @@
         <v>142</v>
       </c>
       <c r="C119" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D119" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2960,10 +2954,10 @@
         <v>131</v>
       </c>
       <c r="C120" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D120" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2971,13 +2965,13 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C121" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D121" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2985,13 +2979,13 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C122" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D122" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3002,10 +2996,10 @@
         <v>131</v>
       </c>
       <c r="C123" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D123" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3016,10 +3010,10 @@
         <v>142</v>
       </c>
       <c r="C124" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D124" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3030,10 +3024,10 @@
         <v>131</v>
       </c>
       <c r="C125" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D125" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3041,13 +3035,13 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D126" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3055,13 +3049,13 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D127" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3069,13 +3063,13 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C128" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D128" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3086,10 +3080,10 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D129" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>